<commit_message>
created contact us model
</commit_message>
<xml_diff>
--- a/design/web_services_api.xlsx
+++ b/design/web_services_api.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
   <si>
     <t>Uri</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>/api/categories</t>
-  </si>
-  <si>
-    <t>/search</t>
   </si>
   <si>
     <t>All winners.</t>
@@ -338,12 +335,33 @@
 required
 </t>
   </si>
+  <si>
+    <t>/api/search</t>
+  </si>
+  <si>
+    <t>key = nullbale ,  key is name setting.</t>
+  </si>
+  <si>
+    <t>return all settings if request = /settings,   return one setting if request = /settings/key</t>
+  </si>
+  <si>
+    <t>/api/contact-us</t>
+  </si>
+  <si>
+    <t>/api/settings/{key?}</t>
+  </si>
+  <si>
+    <t>name = string, email = email, message = string</t>
+  </si>
+  <si>
+    <t>return errors validations or success message</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +406,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -415,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -473,11 +497,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -533,46 +583,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -815,6 +843,40 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
@@ -833,15 +895,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0" headerRowDxfId="0" dataDxfId="7">
-  <autoFilter ref="A1:F29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F31"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Uri" dataDxfId="6"/>
-    <tableColumn id="2" name="Method" dataDxfId="5"/>
-    <tableColumn id="3" name="Parameters" dataDxfId="4"/>
-    <tableColumn id="4" name="Auth" dataDxfId="3"/>
-    <tableColumn id="5" name="Return" dataDxfId="2"/>
-    <tableColumn id="6" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" name="Uri" dataDxfId="5"/>
+    <tableColumn id="2" name="Method" dataDxfId="4"/>
+    <tableColumn id="3" name="Parameters" dataDxfId="3"/>
+    <tableColumn id="4" name="Auth" dataDxfId="2"/>
+    <tableColumn id="5" name="Return" dataDxfId="1"/>
+    <tableColumn id="6" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1134,20 +1196,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="17" style="9" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="64.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="59.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="82.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" style="9" customWidth="1"/>
     <col min="7" max="9" width="9.140625" style="9"/>
     <col min="10" max="10" width="11.5703125" style="9" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="9"/>
@@ -1226,7 +1288,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -1242,7 +1304,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -1254,13 +1316,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3"/>
     </row>
@@ -1272,13 +1334,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1290,13 +1352,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -1312,7 +1374,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -1324,16 +1386,16 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1344,13 +1406,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -1362,13 +1424,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -1384,297 +1446,333 @@
         <v>8</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:15" s="5" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="23"/>
+    </row>
+    <row r="16" spans="1:15" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" s="13" customFormat="1" ht="283.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" s="13" customFormat="1" ht="283.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="B17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="F18" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="13" customFormat="1" ht="189" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" s="13" customFormat="1" ht="236.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" s="13" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="13" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" s="13" customFormat="1" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" s="13" customFormat="1" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="10" t="s">
+    </row>
+    <row r="23" spans="1:6" s="18" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="18" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="B25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6" s="18" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="1:6" s="18" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" s="18" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>68</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>77</v>
+      <c r="C26" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" s="18" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="18" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" s="18" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>79</v>
+      <c r="C28" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="18" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="D29" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated contact up model = added phone in model
</commit_message>
<xml_diff>
--- a/design/web_services_api.xlsx
+++ b/design/web_services_api.xlsx
@@ -351,10 +351,10 @@
     <t>/api/settings/{key?}</t>
   </si>
   <si>
-    <t>name = string, email = email, message = string</t>
-  </si>
-  <si>
     <t>return errors validations or success message</t>
+  </si>
+  <si>
+    <t>name = string, email = email, phone = number, message = string</t>
   </si>
 </sst>
 </file>
@@ -1198,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:15" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="13" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>83</v>
       </c>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="F15" s="23"/>
     </row>
-    <row r="16" spans="1:15" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="13" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>82</v>
       </c>
@@ -1494,13 +1494,13 @@
         <v>19</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="F16" s="23"/>
     </row>

</xml_diff>